<commit_message>
Acrescentando Relacionamentos / PKs e Fks
</commit_message>
<xml_diff>
--- a/BiblioExcel.xlsx
+++ b/BiblioExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arley.saugusto\Documents\REPOS_TURMAS\SenaBiblio-TII01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FCE995-4730-4A80-BB8D-23D9AAFAFD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02DE386-6B29-48C2-B45D-0CC62B3F8E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1F8359A8-2DF1-47F7-AEA5-40A3860C4D23}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>Aluno</t>
   </si>
@@ -77,9 +77,6 @@
     <t>nomeLivro</t>
   </si>
   <si>
-    <t>nomeUsuario</t>
-  </si>
-  <si>
     <t>multa</t>
   </si>
   <si>
@@ -110,18 +107,6 @@
     <t>edicao</t>
   </si>
   <si>
-    <t>Isabela</t>
-  </si>
-  <si>
-    <t>isa12345</t>
-  </si>
-  <si>
-    <t>bla bla</t>
-  </si>
-  <si>
-    <t>bla</t>
-  </si>
-  <si>
     <t>nomeLog</t>
   </si>
   <si>
@@ -140,25 +125,40 @@
     <t>cep</t>
   </si>
   <si>
-    <t>Avenida</t>
-  </si>
-  <si>
-    <t>das Margaridas</t>
-  </si>
-  <si>
-    <t>ap 21</t>
-  </si>
-  <si>
     <t>tipoLog</t>
   </si>
   <si>
     <t>contatoAlternativo</t>
   </si>
   <si>
-    <t>Eugênio</t>
-  </si>
-  <si>
-    <t>null</t>
+    <t>lorem</t>
+  </si>
+  <si>
+    <t>Juquinha</t>
+  </si>
+  <si>
+    <t>Regina</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>PHP Biblia</t>
+  </si>
+  <si>
+    <t>idAluno</t>
+  </si>
+  <si>
+    <t>idEmprestimo</t>
+  </si>
+  <si>
+    <t>idLivro</t>
+  </si>
+  <si>
+    <t>Mariazinha Castro</t>
   </si>
 </sst>
 </file>
@@ -188,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -212,12 +212,23 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -226,21 +237,19 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,251 +585,333 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0502ED4-6F6A-4B0B-968D-2F672D1F3156}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <v>11122233355</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4">
+        <v>77788899900</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3">
+        <v>45296</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45303</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3">
+        <v>45297</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45306</v>
+      </c>
+      <c r="D17" s="3">
+        <v>45304</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="6"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3">
-        <v>11122233344</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3">
-        <v>13988776655</v>
-      </c>
-      <c r="F3">
-        <v>13988776611</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3">
-        <v>123</v>
-      </c>
-      <c r="L3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3">
-        <v>9090</v>
-      </c>
-      <c r="N3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="6">
-        <v>13922337788</v>
-      </c>
-      <c r="F4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="H25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A14:M14"/>
+    <mergeCell ref="A24:M24"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>